<commit_message>
Final copy of PCB rework
</commit_message>
<xml_diff>
--- a/Electrical/Electrical Parts List.xlsx
+++ b/Electrical/Electrical Parts List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\JPL Open Source Rover\open-source-rover\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\Documents\GitHub\open-source-rover\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{325337E2-E5E2-48FC-9E32-9A8A4C218D44}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="141">
   <si>
     <t>Part</t>
   </si>
@@ -420,14 +421,41 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT22K0/CF14JT22K0CT-ND/1830383</t>
+  </si>
+  <si>
+    <t>Jaycar</t>
+  </si>
+  <si>
+    <t>Already have</t>
+  </si>
+  <si>
+    <t>US DIGITAL</t>
+  </si>
+  <si>
+    <t>Digital DC Power Meter with Internal Shunt (MS6170)</t>
+  </si>
+  <si>
+    <t>Universal Professional Balance Charger/Discharger (MB3633)</t>
+  </si>
+  <si>
+    <t>6mm x2m (4 of) (WH5630)</t>
+  </si>
+  <si>
+    <t>Seeed</t>
+  </si>
+  <si>
+    <t>ebay</t>
+  </si>
+  <si>
+    <t>Deans Connector x2 (PT4450)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -504,7 +532,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +542,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -574,7 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -583,9 +641,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -595,9 +650,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -607,9 +659,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -618,9 +667,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -630,22 +676,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -663,49 +709,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -715,7 +746,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -729,6 +760,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1010,1400 +1074,1556 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" customWidth="1"/>
-    <col min="2" max="6" width="14.73046875" customWidth="1"/>
-    <col min="7" max="7" width="17.1328125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.73046875" customWidth="1"/>
-    <col min="10" max="10" width="17.19921875" customWidth="1"/>
-    <col min="11" max="11" width="52.19921875" customWidth="1"/>
+    <col min="1" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="K1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="4">
         <v>735</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="20">
+      <c r="J2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="16">
         <v>1.5</v>
       </c>
-      <c r="J2" s="20">
+      <c r="L2" s="16">
         <v>3</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="M2" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="22">
+      <c r="J3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="18">
         <v>34.99</v>
       </c>
-      <c r="J3" s="22">
+      <c r="L3" s="18">
         <v>34.99</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="M3" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="B4" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="I4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="24">
+      <c r="J4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="20">
         <v>25</v>
       </c>
-      <c r="J4" s="24">
+      <c r="L4" s="20">
         <v>25</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="M4" s="21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="B5" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="22">
+      <c r="J5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="18">
         <v>13.24</v>
       </c>
-      <c r="J5" s="22">
+      <c r="L5" s="18">
         <v>13.24</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="M5" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="B6" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="I6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="22">
+      <c r="J6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="18">
         <v>9.98</v>
       </c>
-      <c r="J6" s="22">
+      <c r="L6" s="18">
         <v>9.98</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="M6" s="19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="12">
-        <v>1</v>
-      </c>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="H7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="I7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="24">
+      <c r="J7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="20">
         <v>6.79</v>
       </c>
-      <c r="J7" s="24">
+      <c r="L7" s="20">
         <v>6.79</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="M7" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="16">
-        <v>1</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="B8" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="H8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="I8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="22">
+      <c r="J8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="18">
         <v>5.57</v>
       </c>
-      <c r="J8" s="22">
+      <c r="L8" s="18">
         <v>5.57</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="M8" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="16">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="B9" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="22">
+      <c r="J9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="18">
         <v>86.95</v>
       </c>
-      <c r="J9" s="22">
+      <c r="L9" s="18">
         <v>86.95</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="M9" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="B10" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="22">
+      <c r="J10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="18">
         <v>41.95</v>
       </c>
-      <c r="J10" s="22">
+      <c r="L10" s="18">
         <v>41.95</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="M10" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:15" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="6">
         <v>25</v>
       </c>
-      <c r="C11" s="8">
+      <c r="E11" s="6">
         <v>4</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="12">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="H11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="I11" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="22">
+      <c r="J11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="18">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="J11" s="22">
-        <f>B11/D11*I11</f>
+      <c r="L11" s="18">
+        <f>D11/F11*K11</f>
         <v>0.72</v>
       </c>
-      <c r="K11" s="53" t="s">
+      <c r="M11" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="M11" s="54"/>
-    </row>
-    <row r="12" spans="1:13" s="55" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="7" t="s">
+      <c r="O11" s="45"/>
+    </row>
+    <row r="12" spans="1:15" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="48"/>
+      <c r="D12" s="6">
         <v>25</v>
       </c>
-      <c r="C12" s="8">
+      <c r="E12" s="6">
         <v>4</v>
       </c>
-      <c r="D12" s="16">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="H12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="52" t="s">
+      <c r="I12" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="22">
+      <c r="J12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="18">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="J12" s="22">
-        <f>B12/D12*I12</f>
+      <c r="L12" s="18">
+        <f>D12/F12*K12</f>
         <v>0.72</v>
       </c>
-      <c r="K12" s="56" t="s">
+      <c r="M12" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="M12" s="54"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="7" t="s">
+      <c r="O12" s="45"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1</v>
-      </c>
-      <c r="D13" s="16">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="B13" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="C13" s="48"/>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="22">
+      <c r="J13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="18">
         <v>24.95</v>
       </c>
-      <c r="J13" s="22">
+      <c r="L13" s="18">
         <v>24.95</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="M13" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="17">
-        <v>1</v>
-      </c>
-      <c r="C14" s="17">
-        <v>1</v>
-      </c>
-      <c r="D14" s="16">
-        <v>1</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="B14" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="H14" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="I14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="22">
+      <c r="J14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="18">
         <v>4.49</v>
       </c>
-      <c r="J14" s="22">
+      <c r="L14" s="18">
         <v>4.49</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="M14" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="48"/>
+      <c r="D15" s="6">
         <v>5</v>
       </c>
-      <c r="C15" s="8">
+      <c r="E15" s="6">
         <v>5</v>
       </c>
-      <c r="D15" s="16">
-        <v>1</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="H15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="I15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="22">
+      <c r="J15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="18">
         <v>69.95</v>
       </c>
-      <c r="J15" s="22">
+      <c r="L15" s="18">
         <v>349.75</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="M15" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="B16" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="I16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="22">
+      <c r="J16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="18">
         <v>14.95</v>
       </c>
-      <c r="J16" s="22">
+      <c r="L16" s="18">
         <v>14.95</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="M16" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="6">
         <v>6</v>
       </c>
-      <c r="C17" s="8">
+      <c r="E17" s="6">
         <v>6</v>
       </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="12">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="I17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="22">
+      <c r="J17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="18">
         <v>34.950000000000003</v>
       </c>
-      <c r="J17" s="22">
+      <c r="L17" s="18">
         <v>209.70000000000002</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="M17" s="19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="6">
         <v>4</v>
       </c>
-      <c r="C18" s="8">
+      <c r="E18" s="6">
         <v>4</v>
       </c>
-      <c r="D18" s="16">
-        <v>1</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="F18" s="12">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="H18" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="I18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="22">
+      <c r="J18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="18">
         <v>19.95</v>
       </c>
-      <c r="J18" s="22">
+      <c r="L18" s="18">
         <v>79.8</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="M18" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="6">
         <v>4</v>
       </c>
-      <c r="C19" s="8">
+      <c r="E19" s="6">
         <v>4</v>
       </c>
-      <c r="D19" s="16">
-        <v>1</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="12">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="H19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="I19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="22">
+      <c r="J19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="18">
         <v>6.8</v>
       </c>
-      <c r="J19" s="22">
+      <c r="L19" s="18">
         <v>27.2</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="M19" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="6">
         <v>4</v>
       </c>
-      <c r="C20" s="8">
+      <c r="E20" s="6">
         <v>4</v>
       </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="F20" s="12">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="H20" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="I20" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="35">
+      <c r="J20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="29">
         <v>55</v>
       </c>
-      <c r="J20" s="22">
+      <c r="L20" s="18">
         <v>220</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="M20" s="19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="17">
-        <v>1</v>
-      </c>
-      <c r="C21" s="17">
-        <v>1</v>
-      </c>
-      <c r="D21" s="16">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="B21" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="13">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13">
+        <v>1</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="H21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="I21" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="22">
+      <c r="J21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="18">
         <v>6.32</v>
       </c>
-      <c r="J21" s="22">
+      <c r="L21" s="18">
         <v>6.32</v>
       </c>
-      <c r="K21" s="27" t="s">
+      <c r="M21" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="17">
-        <v>1</v>
-      </c>
-      <c r="C22" s="17">
-        <v>1</v>
-      </c>
-      <c r="D22" s="16">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17" t="s">
+      <c r="B22" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="13">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1</v>
+      </c>
+      <c r="F22" s="12">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="H22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="I22" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="22">
+      <c r="J22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="18">
         <v>6.14</v>
       </c>
-      <c r="J22" s="22">
+      <c r="L22" s="18">
         <v>6.14</v>
       </c>
-      <c r="K22" s="27" t="s">
+      <c r="M22" s="23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="17">
-        <v>1</v>
-      </c>
-      <c r="C23" s="17">
-        <v>1</v>
-      </c>
-      <c r="D23" s="16">
-        <v>1</v>
-      </c>
-      <c r="E23" s="17" t="s">
+      <c r="B23" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="13">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1</v>
+      </c>
+      <c r="F23" s="12">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="H23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="I23" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="22">
+      <c r="J23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="18">
         <v>4.95</v>
       </c>
-      <c r="J23" s="22">
+      <c r="L23" s="18">
         <v>4.95</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="M23" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="17">
-        <v>1</v>
-      </c>
-      <c r="C24" s="17">
-        <v>1</v>
-      </c>
-      <c r="D24" s="16">
-        <v>1</v>
-      </c>
-      <c r="E24" s="17" t="s">
+      <c r="B24" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="48"/>
+      <c r="D24" s="13">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <v>1</v>
+      </c>
+      <c r="F24" s="12">
+        <v>1</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="H24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="I24" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="22">
+      <c r="J24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="18">
         <v>4.95</v>
       </c>
-      <c r="J24" s="22">
+      <c r="L24" s="18">
         <v>4.95</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="M24" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="17">
-        <v>1</v>
-      </c>
-      <c r="C25" s="17">
-        <v>1</v>
-      </c>
-      <c r="D25" s="16">
-        <v>1</v>
-      </c>
-      <c r="E25" s="17" t="s">
+      <c r="B25" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="13">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13">
+        <v>1</v>
+      </c>
+      <c r="F25" s="12">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="H25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="I25" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="22">
+      <c r="J25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="18">
         <v>4.95</v>
       </c>
-      <c r="J25" s="22">
+      <c r="L25" s="18">
         <v>4.95</v>
       </c>
-      <c r="K25" s="17" t="s">
+      <c r="M25" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="17">
-        <v>1</v>
-      </c>
-      <c r="C26" s="17">
-        <v>1</v>
-      </c>
-      <c r="D26" s="16">
-        <v>1</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="B26" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="48"/>
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13">
+        <v>1</v>
+      </c>
+      <c r="F26" s="12">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="H26" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="I26" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="22">
+      <c r="J26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" s="18">
         <v>4.95</v>
       </c>
-      <c r="J26" s="22">
+      <c r="L26" s="18">
         <v>4.95</v>
       </c>
-      <c r="K26" s="17" t="s">
+      <c r="M26" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" s="30" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="13">
         <v>10</v>
       </c>
-      <c r="C27" s="17">
+      <c r="E27" s="13">
         <v>4</v>
       </c>
-      <c r="D27" s="16">
-        <v>1</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="F27" s="12">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="31" t="s">
+      <c r="H27" s="13"/>
+      <c r="I27" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="22">
+      <c r="J27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="18">
         <v>0.36699999999999999</v>
       </c>
-      <c r="J27" s="22">
+      <c r="L27" s="18">
         <v>3.67</v>
       </c>
-      <c r="K27" s="36" t="s">
+      <c r="M27" s="30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="32" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="58"/>
+      <c r="D28" s="27">
         <v>10</v>
       </c>
-      <c r="C28" s="33">
-        <v>1</v>
-      </c>
-      <c r="D28" s="16">
-        <v>1</v>
-      </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="27">
+        <v>1</v>
+      </c>
+      <c r="F28" s="12">
+        <v>1</v>
+      </c>
+      <c r="G28" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="34" t="s">
+      <c r="H28" s="27"/>
+      <c r="I28" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="37">
+      <c r="J28" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="31">
         <v>0.04</v>
       </c>
-      <c r="J28" s="37">
+      <c r="L28" s="31">
         <v>0.4</v>
       </c>
-      <c r="K28" s="38" t="s">
+      <c r="M28" s="32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" s="39" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="33">
-        <v>1</v>
-      </c>
-      <c r="C29" s="33">
-        <v>1</v>
-      </c>
-      <c r="D29" s="16">
-        <v>1</v>
-      </c>
-      <c r="E29" s="33" t="s">
+      <c r="B29" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="54"/>
+      <c r="D29" s="27">
+        <v>1</v>
+      </c>
+      <c r="E29" s="27">
+        <v>1</v>
+      </c>
+      <c r="F29" s="12">
+        <v>1</v>
+      </c>
+      <c r="G29" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="40" t="s">
+      <c r="H29" s="27"/>
+      <c r="I29" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="37">
+      <c r="J29" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="31">
         <v>7.99</v>
       </c>
-      <c r="J29" s="37">
+      <c r="L29" s="31">
         <v>7.99</v>
       </c>
-      <c r="K29" s="46" t="s">
+      <c r="M29" s="37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A30" s="39" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="33">
-        <v>1</v>
-      </c>
-      <c r="C30" s="33">
-        <v>1</v>
-      </c>
-      <c r="D30" s="16">
-        <v>1</v>
-      </c>
-      <c r="E30" s="33" t="s">
+      <c r="B30" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="54"/>
+      <c r="D30" s="27">
+        <v>1</v>
+      </c>
+      <c r="E30" s="27">
+        <v>1</v>
+      </c>
+      <c r="F30" s="12">
+        <v>1</v>
+      </c>
+      <c r="G30" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="40" t="s">
+      <c r="H30" s="27"/>
+      <c r="I30" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="H30" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="37">
+      <c r="J30" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="31">
         <v>15.59</v>
       </c>
-      <c r="J30" s="37">
+      <c r="L30" s="31">
         <v>15.59</v>
       </c>
-      <c r="K30" s="46" t="s">
+      <c r="M30" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A31" s="39" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="33">
-        <v>1</v>
-      </c>
-      <c r="C31" s="33">
-        <v>1</v>
-      </c>
-      <c r="D31" s="16">
-        <v>1</v>
-      </c>
-      <c r="E31" s="33" t="s">
+      <c r="B31" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="27">
+        <v>1</v>
+      </c>
+      <c r="E31" s="27">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1</v>
+      </c>
+      <c r="G31" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="40" t="s">
+      <c r="H31" s="27"/>
+      <c r="I31" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="H31" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="37">
+      <c r="J31" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="31">
         <v>12.56</v>
       </c>
-      <c r="J31" s="37">
+      <c r="L31" s="31">
         <v>12.56</v>
       </c>
-      <c r="K31" s="47" t="s">
+      <c r="M31" s="38" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A32" s="39" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="33">
-        <v>1</v>
-      </c>
-      <c r="C32" s="33">
-        <v>1</v>
-      </c>
-      <c r="D32" s="16">
-        <v>1</v>
-      </c>
-      <c r="E32" s="33" t="s">
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="27">
+        <v>1</v>
+      </c>
+      <c r="F32" s="12">
+        <v>1</v>
+      </c>
+      <c r="G32" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="40" t="s">
+      <c r="H32" s="27"/>
+      <c r="I32" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="H32" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="37">
+      <c r="J32" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="31">
         <v>15.59</v>
       </c>
-      <c r="J32" s="37">
+      <c r="L32" s="31">
         <v>15.59</v>
       </c>
-      <c r="K32" s="46" t="s">
+      <c r="M32" s="37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A33" s="39" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="16">
-        <v>1</v>
-      </c>
-      <c r="E33" s="33" t="s">
+      <c r="B33" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="49"/>
+      <c r="D33" s="27">
+        <v>1</v>
+      </c>
+      <c r="E33" s="27">
+        <v>1</v>
+      </c>
+      <c r="F33" s="12">
+        <v>1</v>
+      </c>
+      <c r="G33" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="40" t="s">
+      <c r="H33" s="27"/>
+      <c r="I33" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="37">
+      <c r="J33" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="31">
         <v>15.59</v>
       </c>
-      <c r="J33" s="37">
+      <c r="L33" s="31">
         <v>15.59</v>
       </c>
-      <c r="K33" s="46" t="s">
+      <c r="M33" s="37" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A34" s="11" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="48"/>
+      <c r="D34" s="9">
         <v>5</v>
       </c>
-      <c r="C34" s="12">
-        <v>1</v>
-      </c>
-      <c r="D34" s="12">
-        <v>1</v>
-      </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="14" t="s">
+      <c r="H34" s="9"/>
+      <c r="I34" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="24">
+      <c r="J34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="20">
         <v>3.95</v>
       </c>
-      <c r="J34" s="24">
+      <c r="L34" s="20">
         <v>19.75</v>
       </c>
-      <c r="K34" s="26" t="s">
+      <c r="M34" s="22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A35" s="41" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="42">
+      <c r="B35" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="56"/>
+      <c r="D35" s="34">
         <v>10</v>
       </c>
-      <c r="C35" s="42">
+      <c r="E35" s="34">
         <v>5</v>
       </c>
-      <c r="D35" s="42">
-        <v>1</v>
-      </c>
-      <c r="E35" s="42" t="s">
+      <c r="F35" s="34">
+        <v>1</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="42"/>
-      <c r="G35" s="13" t="s">
+      <c r="H35" s="34"/>
+      <c r="I35" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H35" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="48">
+      <c r="J35" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="39">
         <v>0.59</v>
       </c>
-      <c r="J35" s="48">
+      <c r="L35" s="39">
         <v>5.8999999999999995</v>
       </c>
-      <c r="K35" s="49" t="s">
+      <c r="M35" s="40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A36" s="41" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="42">
+      <c r="B36" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="55"/>
+      <c r="D36" s="34">
         <v>20</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42">
-        <v>1</v>
-      </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="34"/>
+      <c r="F36" s="34">
+        <v>1</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="42" t="s">
+      <c r="H36" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="I36" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H36" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="48">
+      <c r="J36" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="39">
         <v>0.35</v>
       </c>
-      <c r="J36" s="48">
+      <c r="L36" s="39">
         <v>7</v>
       </c>
-      <c r="K36" s="42" t="s">
+      <c r="M36" s="34" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A37" s="41" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="42">
-        <v>1</v>
-      </c>
-      <c r="C37" s="42">
-        <v>1</v>
-      </c>
-      <c r="D37" s="42">
-        <v>1</v>
-      </c>
-      <c r="E37" s="42" t="s">
+      <c r="B37" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="51"/>
+      <c r="D37" s="34">
+        <v>1</v>
+      </c>
+      <c r="E37" s="34">
+        <v>1</v>
+      </c>
+      <c r="F37" s="34">
+        <v>1</v>
+      </c>
+      <c r="G37" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="42" t="s">
+      <c r="H37" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="I37" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="48">
+      <c r="J37" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="39">
         <v>20.2</v>
       </c>
-      <c r="J37" s="48">
+      <c r="L37" s="39">
         <v>20.2</v>
       </c>
-      <c r="K37" s="25" t="s">
+      <c r="M37" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A38" s="41" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="42">
-        <v>1</v>
-      </c>
-      <c r="C38" s="42">
-        <v>1</v>
-      </c>
-      <c r="D38" s="42">
-        <v>1</v>
-      </c>
-      <c r="E38" s="42" t="s">
+      <c r="B38" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="51"/>
+      <c r="D38" s="34">
+        <v>1</v>
+      </c>
+      <c r="E38" s="34">
+        <v>1</v>
+      </c>
+      <c r="F38" s="34">
+        <v>1</v>
+      </c>
+      <c r="G38" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="H38" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="I38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H38" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="48">
+      <c r="J38" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="39">
         <v>19.649999999999999</v>
       </c>
-      <c r="J38" s="48">
+      <c r="L38" s="39">
         <v>19.649999999999999</v>
       </c>
-      <c r="K38" s="25" t="s">
+      <c r="M38" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A39" s="43" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="44">
+      <c r="B39" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="50"/>
+      <c r="D39" s="35">
         <v>5</v>
       </c>
-      <c r="C39" s="44">
+      <c r="E39" s="35">
         <v>5</v>
       </c>
-      <c r="D39" s="42">
-        <v>1</v>
-      </c>
-      <c r="E39" s="12" t="s">
+      <c r="F39" s="34">
+        <v>1</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="44"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="50">
+      <c r="H39" s="35"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" s="41">
         <v>5.99</v>
       </c>
-      <c r="J39" s="48">
+      <c r="L39" s="39">
         <v>29.950000000000003</v>
       </c>
-      <c r="K39" s="51" t="s">
+      <c r="M39" s="42" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K7" r:id="rId6"/>
-    <hyperlink ref="K8" r:id="rId7"/>
-    <hyperlink ref="K9" r:id="rId8"/>
-    <hyperlink ref="K10" r:id="rId9"/>
-    <hyperlink ref="K15" r:id="rId10"/>
-    <hyperlink ref="K16" r:id="rId11"/>
-    <hyperlink ref="K17" r:id="rId12"/>
-    <hyperlink ref="K18" r:id="rId13"/>
-    <hyperlink ref="K19" r:id="rId14"/>
-    <hyperlink ref="K20" r:id="rId15"/>
-    <hyperlink ref="K21" r:id="rId16"/>
-    <hyperlink ref="K27" r:id="rId17"/>
-    <hyperlink ref="K28" r:id="rId18"/>
-    <hyperlink ref="K29" r:id="rId19"/>
-    <hyperlink ref="K30" r:id="rId20"/>
-    <hyperlink ref="K31" r:id="rId21"/>
-    <hyperlink ref="K32" r:id="rId22"/>
-    <hyperlink ref="K33" r:id="rId23"/>
-    <hyperlink ref="K35" r:id="rId24"/>
-    <hyperlink ref="K37" r:id="rId25"/>
-    <hyperlink ref="K38" r:id="rId26"/>
-    <hyperlink ref="K39" r:id="rId27"/>
-    <hyperlink ref="K11" r:id="rId28"/>
-    <hyperlink ref="K12" r:id="rId29"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="M8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="M10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="M18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="M19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="M20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="M27" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="M28" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="M29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M30" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="M31" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="M33" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M35" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="M37" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M38" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="M39" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M11" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="M12" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>